<commit_message>
add ad8648 and ad8646
</commit_message>
<xml_diff>
--- a/Tools/接口定义统一标准.xlsx
+++ b/Tools/接口定义统一标准.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS485_RS232" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="53">
   <si>
     <t>接口定义</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,6 +227,10 @@
   </si>
   <si>
     <t>从设备RS232接收</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -300,9 +304,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -315,13 +316,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -674,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -694,203 +698,211 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>4</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
         <v>5</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="4"/>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>6</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4">
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
         <v>6</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>7</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4">
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3">
         <v>7</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>8</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4">
+      <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3">
         <v>8</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="4"/>
+      <c r="E12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>9</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>9</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="4"/>
+      <c r="E13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
@@ -903,189 +915,199 @@
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>1</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3">
         <v>1</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>2</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>3</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>3</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>4</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3">
         <v>4</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>5</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4">
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3">
         <v>5</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="4"/>
+      <c r="E24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>6</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4">
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
         <v>6</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="E25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>7</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4">
+      <c r="B26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3">
         <v>7</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="E26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>8</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4">
+      <c r="B27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3">
         <v>8</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="4"/>
+      <c r="E27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>9</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>9</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="4"/>
+      <c r="E28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A16:F16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="A18:C18"/>
@@ -1094,8 +1116,6 @@
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A16:F16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1106,7 +1126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032B3AEE-B820-47D5-9D41-942231A8302C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -1127,486 +1147,486 @@
       <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>4</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>5</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>6</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>6</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>7</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>7</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>8</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>8</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>9</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>9</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>10</v>
-      </c>
-      <c r="B14" s="8" t="s">
+    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4">
-        <v>10</v>
-      </c>
-      <c r="E14" s="8" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3">
+        <v>10</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
         <v>11</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
         <v>11</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
         <v>12</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3">
         <v>12</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
         <v>13</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3">
         <v>13</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>14</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>14</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
         <v>15</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4">
+      <c r="B19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3">
         <v>15</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="E19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>16</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4">
+      <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3">
         <v>16</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="E20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>17</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4">
+      <c r="B21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3">
         <v>17</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="E21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>18</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3">
         <v>18</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <v>19</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3">
         <v>19</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
         <v>20</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3">
         <v>20</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
         <v>21</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4">
+      <c r="B25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
         <v>21</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="E25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
         <v>22</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4">
+      <c r="B26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3">
         <v>22</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+      <c r="E26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
         <v>23</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4">
+      <c r="B27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3">
         <v>23</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
         <v>24</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>24</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
         <v>25</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="4">
+      <c r="C29" s="8"/>
+      <c r="D29" s="3">
         <v>25</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="F28:F29"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="F28:F29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>